<commit_message>
Working on replicating stats PDF
</commit_message>
<xml_diff>
--- a/documentation/database schema/Features Specifications.xlsx
+++ b/documentation/database schema/Features Specifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="FeatureSpecifications" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="543">
   <si>
     <t>feature_field</t>
   </si>
@@ -1613,6 +1613,42 @@
   </si>
   <si>
     <t>HMM, THAT'S TOO MUCH I THINK.</t>
+  </si>
+  <si>
+    <t>Feature_ID</t>
+  </si>
+  <si>
+    <t>motion_type</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>Actual feature data table</t>
+  </si>
+  <si>
+    <t>CV version number</t>
+  </si>
+  <si>
+    <t>CV algorithm name</t>
+  </si>
+  <si>
+    <t>Batch ID</t>
+  </si>
+  <si>
+    <t>Batch Table</t>
+  </si>
+  <si>
+    <t>feature analysis version number</t>
+  </si>
+  <si>
+    <t>AHA -&gt; that means we can load all the old data!</t>
+  </si>
+  <si>
+    <t>create a little utility to crawl through the files and add all the data</t>
+  </si>
+  <si>
+    <t>then create a utility that kicks off the process of creating a new batch for the new data.</t>
   </si>
 </sst>
 </file>
@@ -2021,11 +2057,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB96"/>
+  <dimension ref="A1:AA118"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB96" sqref="AB96"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,7 +2087,7 @@
     <col min="26" max="26" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>323</v>
       </c>
@@ -2134,7 +2170,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2180,16 +2216,16 @@
       <c r="S2" t="s">
         <v>184</v>
       </c>
+      <c r="Z2">
+        <f t="shared" ref="Z2:Z33" si="0">IF(B2="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA2">
-        <f t="shared" ref="AA2:AA4" si="0">IF(Z2=1,4,1)*IF(Q2=1,4,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <f t="shared" ref="AB2:AB4" si="1">(Z2*3+1)*(Q2*3+1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z2*3+1)*(Q2*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2235,16 +2271,16 @@
       <c r="S3" t="s">
         <v>184</v>
       </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="AA3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB3">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" ref="AA3:AA66" si="1">(Z3*3+1)*(Q3*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>3</v>
@@ -2291,16 +2327,16 @@
       <c r="S4" t="s">
         <v>184</v>
       </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="AA4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A68" si="2">A4+1</f>
         <v>4</v>
@@ -2347,26 +2383,16 @@
       <c r="S5" t="s">
         <v>184</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <f>W5*3+1</f>
-        <v>1</v>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="AA5">
-        <f>IF(Z5=1,4,1)*IF(Q5=1,4,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AB5">
-        <f>(Z5*3+1)*(Q5*3+1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -2410,29 +2436,16 @@
       <c r="S6" t="s">
         <v>161</v>
       </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6">
+      <c r="Z6">
+        <f>IF(B6="movement",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Y6">
-        <f>W6*3+1</f>
-        <v>4</v>
-      </c>
-      <c r="Z6">
-        <v>1</v>
-      </c>
-      <c r="AA6">
-        <f>IF(Z6=1,4,1)*IF(Q6=1,4,1)</f>
-        <v>4</v>
-      </c>
-      <c r="AB6">
-        <f t="shared" ref="AB6:AB69" si="3">(Z6*3+1)*(Q6*3+1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -2480,18 +2493,15 @@
         <v>161</v>
       </c>
       <c r="Z7">
+        <f t="shared" ref="Z7:Z70" si="3">IF(B7="movement",1,0)</f>
         <v>1</v>
       </c>
       <c r="AA7">
-        <f t="shared" ref="AA7:AA70" si="4">IF(Z7=1,4,1)*IF(Q7=1,4,1)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB7">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -2539,18 +2549,15 @@
         <v>161</v>
       </c>
       <c r="Z8">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB8">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -2598,18 +2605,15 @@
         <v>161</v>
       </c>
       <c r="Z9">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB9">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -2654,18 +2658,15 @@
         <v>162</v>
       </c>
       <c r="Z10">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB10">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -2710,18 +2711,15 @@
         <v>161</v>
       </c>
       <c r="Z11">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB11">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -2766,18 +2764,15 @@
         <v>163</v>
       </c>
       <c r="Z12">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB12">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -2828,18 +2823,15 @@
         <v>164</v>
       </c>
       <c r="Z13">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB13">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -2890,18 +2882,15 @@
         <v>164</v>
       </c>
       <c r="Z14">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB14">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -2952,18 +2941,15 @@
         <v>164</v>
       </c>
       <c r="Z15">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB15">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -3014,18 +3000,15 @@
         <v>164</v>
       </c>
       <c r="Z16">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -3076,18 +3059,15 @@
         <v>164</v>
       </c>
       <c r="Z17">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB17">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -3138,18 +3118,15 @@
         <v>164</v>
       </c>
       <c r="Z18">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB18">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -3200,18 +3177,15 @@
         <v>164</v>
       </c>
       <c r="Z19">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB19">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -3262,18 +3236,15 @@
         <v>164</v>
       </c>
       <c r="Z20">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB20">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -3324,18 +3295,15 @@
         <v>164</v>
       </c>
       <c r="Z21">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB21">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -3386,18 +3354,15 @@
         <v>164</v>
       </c>
       <c r="Z22">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB22">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -3445,18 +3410,15 @@
         <v>161</v>
       </c>
       <c r="Z23">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB23">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -3504,18 +3466,15 @@
         <v>163</v>
       </c>
       <c r="Z24">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB24">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -3563,18 +3522,15 @@
         <v>161</v>
       </c>
       <c r="Z25">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB25">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -3622,18 +3578,15 @@
         <v>161</v>
       </c>
       <c r="Z26">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB26">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -3678,18 +3631,15 @@
         <v>161</v>
       </c>
       <c r="Z27">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB27">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -3734,18 +3684,15 @@
         <v>163</v>
       </c>
       <c r="Z28">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB28">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -3790,18 +3737,15 @@
         <v>165</v>
       </c>
       <c r="Z29">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB29">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -3849,18 +3793,15 @@
         <v>164</v>
       </c>
       <c r="Z30">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB30">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -3908,18 +3849,15 @@
         <v>164</v>
       </c>
       <c r="Z31">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB31">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -3967,18 +3905,15 @@
         <v>164</v>
       </c>
       <c r="Z32">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB32">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -4029,18 +3964,15 @@
         <v>0</v>
       </c>
       <c r="Z33">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB33">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -4091,18 +4023,15 @@
         <v>1</v>
       </c>
       <c r="Z34">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB34">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -4153,18 +4082,15 @@
         <v>2</v>
       </c>
       <c r="Z35">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB35">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -4215,18 +4141,15 @@
         <v>3</v>
       </c>
       <c r="Z36">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA36">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB36">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -4277,18 +4200,15 @@
         <v>4</v>
       </c>
       <c r="Z37">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB37">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -4339,18 +4259,15 @@
         <v>5</v>
       </c>
       <c r="Z38">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB38">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>A38+1</f>
         <v>38</v>
@@ -4401,18 +4318,15 @@
         <v>166</v>
       </c>
       <c r="Z39">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB39">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -4463,18 +4377,15 @@
         <v>166</v>
       </c>
       <c r="Z40">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB40">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -4525,18 +4436,15 @@
         <v>166</v>
       </c>
       <c r="Z41">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB41">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -4587,18 +4495,15 @@
         <v>166</v>
       </c>
       <c r="Z42">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB42">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -4649,18 +4554,15 @@
         <v>166</v>
       </c>
       <c r="Z43">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA43">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB43">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -4711,18 +4613,15 @@
         <v>167</v>
       </c>
       <c r="Z44">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA44">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB44">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -4773,18 +4672,15 @@
         <v>167</v>
       </c>
       <c r="Z45">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA45">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB45">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -4835,18 +4731,15 @@
         <v>167</v>
       </c>
       <c r="Z46">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA46">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB46">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -4897,18 +4790,15 @@
         <v>167</v>
       </c>
       <c r="Z47">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA47">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB47">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4959,18 +4849,15 @@
         <v>167</v>
       </c>
       <c r="Z48">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA48">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB48">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -5018,18 +4905,15 @@
         <v>161</v>
       </c>
       <c r="Z49">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA49">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB49">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -5077,18 +4961,15 @@
         <v>167</v>
       </c>
       <c r="Z50">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA50">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB50">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -5139,18 +5020,15 @@
         <v>164</v>
       </c>
       <c r="Z51">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA51">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB51">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -5201,18 +5079,15 @@
         <v>164</v>
       </c>
       <c r="Z52">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA52">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB52">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -5263,18 +5138,15 @@
         <v>164</v>
       </c>
       <c r="Z53">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA53">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB53">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -5325,18 +5197,15 @@
         <v>168</v>
       </c>
       <c r="Z54">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA54">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB54">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -5387,18 +5256,15 @@
         <v>168</v>
       </c>
       <c r="Z55">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA55">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB55">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -5449,18 +5315,15 @@
         <v>168</v>
       </c>
       <c r="Z56">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA56">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB56">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -5508,18 +5371,15 @@
         <v>161</v>
       </c>
       <c r="Z57">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB57">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -5564,18 +5424,15 @@
         <v>169</v>
       </c>
       <c r="Z58">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AA58">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="AB58">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -5634,16 +5491,16 @@
       <c r="X59">
         <v>0</v>
       </c>
+      <c r="Z59">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA59">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AB59">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -5702,16 +5559,16 @@
       <c r="X60">
         <v>0</v>
       </c>
+      <c r="Z60">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA60">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AB60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -5770,16 +5627,16 @@
       <c r="X61">
         <v>0</v>
       </c>
+      <c r="Z61">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA61">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AB61">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="2"/>
         <v>61</v>
@@ -5835,16 +5692,16 @@
       <c r="X62">
         <v>1</v>
       </c>
+      <c r="Z62">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA62">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AB62">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -5900,16 +5757,16 @@
       <c r="X63">
         <v>1</v>
       </c>
+      <c r="Z63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA63">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AB63">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="2"/>
         <v>63</v>
@@ -5974,16 +5831,16 @@
       <c r="X64">
         <v>0</v>
       </c>
+      <c r="Z64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB64">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -6048,16 +5905,16 @@
       <c r="X65">
         <v>0</v>
       </c>
+      <c r="Z65">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB65">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="2"/>
         <v>65</v>
@@ -6122,16 +5979,16 @@
       <c r="X66">
         <v>0</v>
       </c>
+      <c r="Z66">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AB66">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="2"/>
         <v>66</v>
@@ -6190,16 +6047,16 @@
       <c r="X67">
         <v>1</v>
       </c>
+      <c r="Z67">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA67">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AB67">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" ref="AA67:AA94" si="4">(Z67*3+1)*(Q67*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="2"/>
         <v>67</v>
@@ -6258,16 +6115,16 @@
       <c r="X68">
         <v>1</v>
       </c>
+      <c r="Z68">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA68">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="AB68">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" ref="A69:A94" si="5">A68+1</f>
         <v>68</v>
@@ -6332,16 +6189,16 @@
       <c r="X69">
         <v>0</v>
       </c>
+      <c r="Z69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA69">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="AB69">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="5"/>
         <v>69</v>
@@ -6406,16 +6263,16 @@
       <c r="X70">
         <v>0</v>
       </c>
+      <c r="Z70">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AA70">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="AB70">
-        <f t="shared" ref="AB70:AB94" si="6">(Z70*3+1)*(Q70*3+1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="5"/>
         <v>70</v>
@@ -6480,16 +6337,16 @@
       <c r="X71">
         <v>0</v>
       </c>
+      <c r="Z71">
+        <f t="shared" ref="Z71:Z94" si="6">IF(B71="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA71">
-        <f t="shared" ref="AA71:AA94" si="7">IF(Z71=1,4,1)*IF(Q71=1,4,1)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="AB71">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="5"/>
         <v>71</v>
@@ -6548,16 +6405,16 @@
       <c r="X72">
         <v>1</v>
       </c>
+      <c r="Z72">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA72">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB72">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="5"/>
         <v>72</v>
@@ -6616,16 +6473,16 @@
       <c r="X73">
         <v>1</v>
       </c>
+      <c r="Z73">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA73">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB73">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="5"/>
         <v>73</v>
@@ -6687,16 +6544,16 @@
       <c r="X74">
         <v>0</v>
       </c>
+      <c r="Z74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA74">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB74">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="5"/>
         <v>74</v>
@@ -6758,16 +6615,16 @@
       <c r="X75">
         <v>0</v>
       </c>
+      <c r="Z75">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA75">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB75">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="5"/>
         <v>75</v>
@@ -6829,16 +6686,16 @@
       <c r="X76">
         <v>0</v>
       </c>
+      <c r="Z76">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA76">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB76">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="5"/>
         <v>76</v>
@@ -6900,16 +6757,16 @@
       <c r="X77">
         <v>0</v>
       </c>
+      <c r="Z77">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA77">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB77">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="5"/>
         <v>77</v>
@@ -6968,16 +6825,16 @@
       <c r="X78">
         <v>1</v>
       </c>
+      <c r="Z78">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA78">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB78">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="5"/>
         <v>78</v>
@@ -7039,16 +6896,16 @@
       <c r="X79">
         <v>1</v>
       </c>
+      <c r="Z79">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA79">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB79">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="5"/>
         <v>79</v>
@@ -7110,16 +6967,16 @@
       <c r="X80">
         <v>1</v>
       </c>
+      <c r="Z80">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA80">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB80">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="5"/>
         <v>80</v>
@@ -7181,16 +7038,16 @@
       <c r="X81">
         <v>0</v>
       </c>
+      <c r="Z81">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA81">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB81">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="5"/>
         <v>81</v>
@@ -7252,16 +7109,16 @@
       <c r="X82">
         <v>0</v>
       </c>
+      <c r="Z82">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA82">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB82">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="5"/>
         <v>82</v>
@@ -7323,16 +7180,16 @@
       <c r="X83">
         <v>0</v>
       </c>
+      <c r="Z83">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA83">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB83">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="5"/>
         <v>83</v>
@@ -7394,16 +7251,16 @@
       <c r="X84">
         <v>0</v>
       </c>
+      <c r="Z84">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA84">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB84">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="5"/>
         <v>84</v>
@@ -7462,16 +7319,16 @@
       <c r="X85">
         <v>1</v>
       </c>
+      <c r="Z85">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA85">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB85">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="5"/>
         <v>85</v>
@@ -7533,16 +7390,16 @@
       <c r="X86">
         <v>1</v>
       </c>
+      <c r="Z86">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA86">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB86">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="5"/>
         <v>86</v>
@@ -7604,16 +7461,16 @@
       <c r="X87">
         <v>1</v>
       </c>
+      <c r="Z87">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA87">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB87">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="5"/>
         <v>87</v>
@@ -7675,16 +7532,16 @@
       <c r="X88">
         <v>0</v>
       </c>
+      <c r="Z88">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA88">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB88">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="5"/>
         <v>88</v>
@@ -7746,16 +7603,16 @@
       <c r="X89">
         <v>0</v>
       </c>
+      <c r="Z89">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA89">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB89">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="5"/>
         <v>89</v>
@@ -7817,16 +7674,16 @@
       <c r="X90">
         <v>0</v>
       </c>
+      <c r="Z90">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA90">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB90">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="5"/>
         <v>90</v>
@@ -7888,16 +7745,16 @@
       <c r="X91">
         <v>0</v>
       </c>
+      <c r="Z91">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA91">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB91">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="5"/>
         <v>91</v>
@@ -7956,16 +7813,16 @@
       <c r="X92">
         <v>1</v>
       </c>
+      <c r="Z92">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA92">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB92">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="5"/>
         <v>92</v>
@@ -8027,16 +7884,16 @@
       <c r="X93">
         <v>1</v>
       </c>
+      <c r="Z93">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA93">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB93">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="5"/>
         <v>93</v>
@@ -8098,23 +7955,84 @@
       <c r="X94">
         <v>1</v>
       </c>
+      <c r="Z94">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AA94">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AB94">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="AA96" s="1">
         <f>SUM(AA2:AA94)</f>
         <v>726</v>
       </c>
-      <c r="AB96" s="1">
-        <f>SUM(AB2:AB94)</f>
-        <v>726</v>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -8127,8 +8045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added a seaborn plot
</commit_message>
<xml_diff>
--- a/documentation/database schema/Features Specifications.xlsx
+++ b/documentation/database schema/Features Specifications.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="588">
   <si>
     <t>feature_field</t>
   </si>
@@ -2247,11 +2247,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB94"/>
+  <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,11 +2274,10 @@
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>323</v>
       </c>
@@ -2355,16 +2354,13 @@
         <v>12</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2416,16 +2412,16 @@
       <c r="T2" s="6" t="s">
         <v>184</v>
       </c>
+      <c r="Z2" s="6">
+        <f>IF(B2="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA2" s="6">
-        <f t="shared" ref="AA2:AA33" si="0">IF(B2="movement",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB2" s="6">
-        <f>(AA2*3+1)*(R2*3+1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(Z2*3+1)*(R2*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2477,16 +2473,16 @@
       <c r="T3" s="6" t="s">
         <v>184</v>
       </c>
+      <c r="Z3" s="6">
+        <f>IF(B3="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="6">
-        <f t="shared" ref="AB3:AB66" si="1">(AA3*3+1)*(R3*3+1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(Z3*3+1)*(R3*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f>A3+1</f>
         <v>3</v>
@@ -2539,18 +2535,18 @@
       <c r="T4" s="6" t="s">
         <v>184</v>
       </c>
+      <c r="Z4" s="6">
+        <f>IF(B4="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA4" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(Z4*3+1)*(R4*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <f t="shared" ref="A5:A68" si="2">A4+1</f>
+        <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2601,18 +2597,18 @@
       <c r="T5" s="6" t="s">
         <v>184</v>
       </c>
+      <c r="Z5" s="6">
+        <f>IF(B5="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA5" s="6">
+        <f>(Z5*3+1)*(R5*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -2662,18 +2658,18 @@
       <c r="T6" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z6" s="6">
+        <f>IF(B6="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA6" s="6">
+        <f>(Z6*3+1)*(R6*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB6" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2725,18 +2721,18 @@
       <c r="T7" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z7" s="6">
+        <f>IF(B7="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA7" s="6">
+        <f>(Z7*3+1)*(R7*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB7" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -2788,18 +2784,18 @@
       <c r="T8" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z8" s="6">
+        <f>IF(B8="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA8" s="6">
+        <f>(Z8*3+1)*(R8*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB8" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -2851,18 +2847,18 @@
       <c r="T9" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z9" s="6">
+        <f>IF(B9="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA9" s="6">
+        <f>(Z9*3+1)*(R9*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB9" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2912,18 +2908,18 @@
       <c r="T10" s="6" t="s">
         <v>162</v>
       </c>
+      <c r="Z10" s="6">
+        <f>IF(B10="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA10" s="6">
+        <f>(Z10*3+1)*(R10*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB10" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -2973,18 +2969,18 @@
       <c r="T11" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z11" s="6">
+        <f>IF(B11="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA11" s="6">
+        <f>(Z11*3+1)*(R11*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB11" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -3034,18 +3030,18 @@
       <c r="T12" s="6" t="s">
         <v>163</v>
       </c>
+      <c r="Z12" s="6">
+        <f>IF(B12="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA12" s="6">
+        <f>(Z12*3+1)*(R12*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB12" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -3099,18 +3095,18 @@
       <c r="T13" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z13" s="6">
+        <f>IF(B13="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA13" s="6">
+        <f>(Z13*3+1)*(R13*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB13" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3164,18 +3160,18 @@
       <c r="T14" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z14" s="6">
+        <f>IF(B14="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA14" s="6">
+        <f>(Z14*3+1)*(R14*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB14" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -3229,18 +3225,18 @@
       <c r="T15" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z15" s="6">
+        <f>IF(B15="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA15" s="6">
+        <f>(Z15*3+1)*(R15*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB15" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -3294,18 +3290,18 @@
       <c r="T16" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z16" s="6">
+        <f>IF(B16="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA16" s="6">
+        <f>(Z16*3+1)*(R16*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB16" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -3359,18 +3355,18 @@
       <c r="T17" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z17" s="6">
+        <f>IF(B17="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA17" s="6">
+        <f>(Z17*3+1)*(R17*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB17" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -3424,18 +3420,18 @@
       <c r="T18" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z18" s="6">
+        <f>IF(B18="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA18" s="6">
+        <f>(Z18*3+1)*(R18*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB18" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -3489,18 +3485,18 @@
       <c r="T19" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z19" s="6">
+        <f>IF(B19="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA19" s="6">
+        <f>(Z19*3+1)*(R19*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB19" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -3554,18 +3550,18 @@
       <c r="T20" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z20" s="6">
+        <f>IF(B20="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA20" s="6">
+        <f>(Z20*3+1)*(R20*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB20" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -3619,18 +3615,18 @@
       <c r="T21" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z21" s="6">
+        <f>IF(B21="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA21" s="6">
+        <f>(Z21*3+1)*(R21*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB21" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -3684,18 +3680,18 @@
       <c r="T22" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z22" s="6">
+        <f>IF(B22="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA22" s="6">
+        <f>(Z22*3+1)*(R22*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB22" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -3747,18 +3743,18 @@
       <c r="T23" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z23" s="6">
+        <f>IF(B23="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA23" s="6">
+        <f>(Z23*3+1)*(R23*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB23" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -3810,18 +3806,18 @@
       <c r="T24" s="6" t="s">
         <v>163</v>
       </c>
+      <c r="Z24" s="6">
+        <f>IF(B24="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA24" s="6">
+        <f>(Z24*3+1)*(R24*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB24" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -3873,18 +3869,18 @@
       <c r="T25" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z25" s="6">
+        <f>IF(B25="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA25" s="6">
+        <f>(Z25*3+1)*(R25*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB25" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -3936,18 +3932,18 @@
       <c r="T26" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z26" s="6">
+        <f>IF(B26="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA26" s="6">
+        <f>(Z26*3+1)*(R26*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB26" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -3997,18 +3993,18 @@
       <c r="T27" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z27" s="6">
+        <f>IF(B27="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA27" s="6">
+        <f>(Z27*3+1)*(R27*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB27" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -4058,18 +4054,18 @@
       <c r="T28" s="6" t="s">
         <v>163</v>
       </c>
+      <c r="Z28" s="6">
+        <f>IF(B28="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA28" s="6">
+        <f>(Z28*3+1)*(R28*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB28" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -4119,18 +4115,18 @@
       <c r="T29" s="6" t="s">
         <v>165</v>
       </c>
+      <c r="Z29" s="6">
+        <f>IF(B29="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA29" s="6">
+        <f>(Z29*3+1)*(R29*3+1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB29" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -4182,18 +4178,18 @@
       <c r="T30" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z30" s="6">
+        <f>IF(B30="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA30" s="6">
+        <f>(Z30*3+1)*(R30*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB30" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -4245,18 +4241,18 @@
       <c r="T31" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z31" s="6">
+        <f>IF(B31="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA31" s="6">
+        <f>(Z31*3+1)*(R31*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB31" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -4308,18 +4304,18 @@
       <c r="T32" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z32" s="6">
+        <f>IF(B32="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA32" s="6">
+        <f>(Z32*3+1)*(R32*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB32" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -4372,20 +4368,17 @@
         <v>163</v>
       </c>
       <c r="Z33" s="6">
-        <v>0</v>
+        <f>IF(B33="movement",1,0)</f>
+        <v>1</v>
       </c>
       <c r="AA33" s="6">
+        <f>(Z33*3+1)*(R33*3+1)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AB33" s="6">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -4438,20 +4431,17 @@
         <v>163</v>
       </c>
       <c r="Z34" s="6">
+        <f>IF(B34="movement",1,0)</f>
         <v>1</v>
       </c>
       <c r="AA34" s="6">
-        <f t="shared" ref="AA34:AA65" si="3">IF(B34="movement",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AB34" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z34*3+1)*(R34*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -4504,20 +4494,17 @@
         <v>163</v>
       </c>
       <c r="Z35" s="6">
-        <v>2</v>
+        <f>IF(B35="movement",1,0)</f>
+        <v>1</v>
       </c>
       <c r="AA35" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB35" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z35*3+1)*(R35*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -4570,20 +4557,17 @@
         <v>163</v>
       </c>
       <c r="Z36" s="6">
-        <v>3</v>
+        <f>IF(B36="movement",1,0)</f>
+        <v>1</v>
       </c>
       <c r="AA36" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB36" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z36*3+1)*(R36*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -4636,20 +4620,17 @@
         <v>163</v>
       </c>
       <c r="Z37" s="6">
-        <v>4</v>
+        <f>IF(B37="movement",1,0)</f>
+        <v>1</v>
       </c>
       <c r="AA37" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB37" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z37*3+1)*(R37*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -4702,18 +4683,15 @@
         <v>163</v>
       </c>
       <c r="Z38" s="6">
-        <v>5</v>
+        <f>IF(B38="movement",1,0)</f>
+        <v>1</v>
       </c>
       <c r="AA38" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB38" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z38*3+1)*(R38*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <f>A38+1</f>
         <v>38</v>
@@ -4769,18 +4747,18 @@
       <c r="T39" s="6" t="s">
         <v>166</v>
       </c>
+      <c r="Z39" s="6">
+        <f>IF(B39="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA39" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB39" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z39*3+1)*(R39*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -4834,18 +4812,18 @@
       <c r="T40" s="6" t="s">
         <v>166</v>
       </c>
+      <c r="Z40" s="6">
+        <f>IF(B40="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA40" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB40" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z40*3+1)*(R40*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -4899,18 +4877,18 @@
       <c r="T41" s="6" t="s">
         <v>166</v>
       </c>
+      <c r="Z41" s="6">
+        <f>IF(B41="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA41" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB41" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z41*3+1)*(R41*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -4964,18 +4942,18 @@
       <c r="T42" s="6" t="s">
         <v>166</v>
       </c>
+      <c r="Z42" s="6">
+        <f>IF(B42="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA42" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB42" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z42*3+1)*(R42*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -5029,18 +5007,18 @@
       <c r="T43" s="6" t="s">
         <v>166</v>
       </c>
+      <c r="Z43" s="6">
+        <f>IF(B43="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA43" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB43" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z43*3+1)*(R43*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -5094,18 +5072,18 @@
       <c r="T44" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="Z44" s="6">
+        <f>IF(B44="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA44" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB44" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z44*3+1)*(R44*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -5159,18 +5137,18 @@
       <c r="T45" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="Z45" s="6">
+        <f>IF(B45="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA45" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB45" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z45*3+1)*(R45*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -5224,18 +5202,18 @@
       <c r="T46" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="Z46" s="6">
+        <f>IF(B46="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA46" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB46" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z46*3+1)*(R46*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5289,18 +5267,18 @@
       <c r="T47" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="Z47" s="6">
+        <f>IF(B47="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA47" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB47" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z47*3+1)*(R47*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -5354,18 +5332,18 @@
       <c r="T48" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="Z48" s="6">
+        <f>IF(B48="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA48" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB48" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z48*3+1)*(R48*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -5417,18 +5395,18 @@
       <c r="T49" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z49" s="6">
+        <f>IF(B49="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA49" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB49" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z49*3+1)*(R49*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -5480,18 +5458,18 @@
       <c r="T50" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="Z50" s="6">
+        <f>IF(B50="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA50" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB50" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z50*3+1)*(R50*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -5545,18 +5523,18 @@
       <c r="T51" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z51" s="6">
+        <f>IF(B51="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA51" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB51" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z51*3+1)*(R51*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
@@ -5610,18 +5588,18 @@
       <c r="T52" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z52" s="6">
+        <f>IF(B52="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA52" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB52" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z52*3+1)*(R52*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -5675,18 +5653,18 @@
       <c r="T53" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="Z53" s="6">
+        <f>IF(B53="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA53" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB53" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z53*3+1)*(R53*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
@@ -5740,18 +5718,18 @@
       <c r="T54" s="6" t="s">
         <v>168</v>
       </c>
+      <c r="Z54" s="6">
+        <f>IF(B54="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA54" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB54" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z54*3+1)*(R54*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
@@ -5805,18 +5783,18 @@
       <c r="T55" s="6" t="s">
         <v>168</v>
       </c>
+      <c r="Z55" s="6">
+        <f>IF(B55="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA55" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB55" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z55*3+1)*(R55*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
@@ -5870,18 +5848,18 @@
       <c r="T56" s="6" t="s">
         <v>168</v>
       </c>
+      <c r="Z56" s="6">
+        <f>IF(B56="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA56" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB56" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z56*3+1)*(R56*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -5933,18 +5911,18 @@
       <c r="T57" s="6" t="s">
         <v>161</v>
       </c>
+      <c r="Z57" s="6">
+        <f>IF(B57="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA57" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB57" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z57*3+1)*(R57*3+1)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
@@ -5994,18 +5972,18 @@
       <c r="T58" s="6" t="s">
         <v>169</v>
       </c>
+      <c r="Z58" s="6">
+        <f>IF(B58="movement",1,0)</f>
+        <v>1</v>
+      </c>
       <c r="AA58" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AB58" s="6">
-        <f t="shared" si="1"/>
+        <f>(Z58*3+1)*(R58*3+1)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -6069,18 +6047,18 @@
       <c r="Y59" s="6">
         <v>0</v>
       </c>
+      <c r="Z59" s="6">
+        <f>IF(B59="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA59" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB59" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(Z59*3+1)*(R59*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
@@ -6144,18 +6122,18 @@
       <c r="Y60" s="6">
         <v>0</v>
       </c>
+      <c r="Z60" s="6">
+        <f>IF(B60="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA60" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB60" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(Z60*3+1)*(R60*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
@@ -6219,18 +6197,18 @@
       <c r="Y61" s="6">
         <v>0</v>
       </c>
+      <c r="Z61" s="6">
+        <f>IF(B61="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA61" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB61" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(Z61*3+1)*(R61*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -6291,18 +6269,18 @@
       <c r="Y62" s="6">
         <v>1</v>
       </c>
+      <c r="Z62" s="6">
+        <f>IF(B62="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA62" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB62" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <f>(Z62*3+1)*(R62*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B63" s="6" t="s">
@@ -6363,18 +6341,18 @@
       <c r="Y63" s="6">
         <v>1</v>
       </c>
+      <c r="Z63" s="6">
+        <f>IF(B63="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA63" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB63" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z63*3+1)*(R63*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
@@ -6440,18 +6418,18 @@
       <c r="Y64">
         <v>0</v>
       </c>
+      <c r="Z64">
+        <f>IF(B64="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB64">
-        <f t="shared" si="1"/>
+        <f>(Z64*3+1)*(R64*3+1)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B65" t="s">
@@ -6517,18 +6495,18 @@
       <c r="Y65">
         <v>0</v>
       </c>
+      <c r="Z65">
+        <f>IF(B65="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA65">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB65">
-        <f t="shared" si="1"/>
+        <f>(Z65*3+1)*(R65*3+1)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="B66" t="s">
@@ -6594,18 +6572,18 @@
       <c r="Y66">
         <v>0</v>
       </c>
+      <c r="Z66">
+        <f>IF(B66="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA66">
-        <f t="shared" ref="AA66:AA94" si="4">IF(B66="movement",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB66">
-        <f t="shared" si="1"/>
+        <f>(Z66*3+1)*(R66*3+1)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B67" t="s">
@@ -6665,18 +6643,18 @@
       <c r="Y67">
         <v>1</v>
       </c>
+      <c r="Z67">
+        <f>IF(B67="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA67">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB67">
-        <f t="shared" ref="AB67:AB94" si="5">(AA67*3+1)*(R67*3+1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z67*3+1)*(R67*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="B68" t="s">
@@ -6736,18 +6714,18 @@
       <c r="Y68">
         <v>1</v>
       </c>
+      <c r="Z68">
+        <f>IF(B68="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA68">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB68">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z68*3+1)*(R68*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" ref="A69:A94" si="6">A68+1</f>
+        <f t="shared" ref="A69:A94" si="1">A68+1</f>
         <v>68</v>
       </c>
       <c r="B69" t="s">
@@ -6813,18 +6791,18 @@
       <c r="Y69">
         <v>0</v>
       </c>
+      <c r="Z69">
+        <f>IF(B69="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA69">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB69">
-        <f t="shared" si="5"/>
+        <f>(Z69*3+1)*(R69*3+1)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="B70" t="s">
@@ -6890,18 +6868,18 @@
       <c r="Y70">
         <v>0</v>
       </c>
+      <c r="Z70">
+        <f>IF(B70="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA70">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB70">
-        <f t="shared" si="5"/>
+        <f>(Z70*3+1)*(R70*3+1)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B71" t="s">
@@ -6967,18 +6945,18 @@
       <c r="Y71">
         <v>0</v>
       </c>
+      <c r="Z71">
+        <f>IF(B71="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA71">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB71">
-        <f t="shared" si="5"/>
+        <f>(Z71*3+1)*(R71*3+1)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="B72" t="s">
@@ -7038,18 +7016,18 @@
       <c r="Y72">
         <v>1</v>
       </c>
+      <c r="Z72">
+        <f>IF(B72="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB72">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z72*3+1)*(R72*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="B73" t="s">
@@ -7109,18 +7087,18 @@
       <c r="Y73">
         <v>1</v>
       </c>
+      <c r="Z73">
+        <f>IF(B73="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA73">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB73">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z73*3+1)*(R73*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="B74" t="s">
@@ -7183,18 +7161,18 @@
       <c r="Y74">
         <v>0</v>
       </c>
+      <c r="Z74">
+        <f>IF(B74="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA74">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB74">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z74*3+1)*(R74*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="B75" t="s">
@@ -7257,18 +7235,18 @@
       <c r="Y75">
         <v>0</v>
       </c>
+      <c r="Z75">
+        <f>IF(B75="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA75">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB75">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z75*3+1)*(R75*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="B76" t="s">
@@ -7331,18 +7309,18 @@
       <c r="Y76">
         <v>0</v>
       </c>
+      <c r="Z76">
+        <f>IF(B76="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA76">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB76">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z76*3+1)*(R76*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="B77" t="s">
@@ -7405,18 +7383,18 @@
       <c r="Y77">
         <v>0</v>
       </c>
+      <c r="Z77">
+        <f>IF(B77="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA77">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB77">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z77*3+1)*(R77*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="B78" t="s">
@@ -7476,18 +7454,18 @@
       <c r="Y78">
         <v>1</v>
       </c>
+      <c r="Z78">
+        <f>IF(B78="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA78">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB78">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z78*3+1)*(R78*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="B79" t="s">
@@ -7550,18 +7528,18 @@
       <c r="Y79">
         <v>1</v>
       </c>
+      <c r="Z79">
+        <f>IF(B79="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA79">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB79">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z79*3+1)*(R79*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>79</v>
       </c>
       <c r="B80" t="s">
@@ -7624,18 +7602,18 @@
       <c r="Y80">
         <v>1</v>
       </c>
+      <c r="Z80">
+        <f>IF(B80="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA80">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB80">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z80*3+1)*(R80*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="B81" t="s">
@@ -7698,18 +7676,18 @@
       <c r="Y81">
         <v>0</v>
       </c>
+      <c r="Z81">
+        <f>IF(B81="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA81">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB81">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z81*3+1)*(R81*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="B82" t="s">
@@ -7772,18 +7750,18 @@
       <c r="Y82">
         <v>0</v>
       </c>
+      <c r="Z82">
+        <f>IF(B82="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA82">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB82">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z82*3+1)*(R82*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="B83" t="s">
@@ -7846,18 +7824,18 @@
       <c r="Y83">
         <v>0</v>
       </c>
+      <c r="Z83">
+        <f>IF(B83="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA83">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB83">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z83*3+1)*(R83*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="B84" t="s">
@@ -7920,18 +7898,18 @@
       <c r="Y84">
         <v>0</v>
       </c>
+      <c r="Z84">
+        <f>IF(B84="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA84">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB84">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z84*3+1)*(R84*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="B85" t="s">
@@ -7991,18 +7969,18 @@
       <c r="Y85">
         <v>1</v>
       </c>
+      <c r="Z85">
+        <f>IF(B85="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA85">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB85">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z85*3+1)*(R85*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="B86" t="s">
@@ -8065,18 +8043,18 @@
       <c r="Y86">
         <v>1</v>
       </c>
+      <c r="Z86">
+        <f>IF(B86="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA86">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB86">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z86*3+1)*(R86*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="B87" t="s">
@@ -8139,18 +8117,18 @@
       <c r="Y87">
         <v>1</v>
       </c>
+      <c r="Z87">
+        <f>IF(B87="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA87">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB87">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z87*3+1)*(R87*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="B88" t="s">
@@ -8213,18 +8191,18 @@
       <c r="Y88">
         <v>0</v>
       </c>
+      <c r="Z88">
+        <f>IF(B88="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA88">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB88">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z88*3+1)*(R88*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="B89" t="s">
@@ -8287,18 +8265,18 @@
       <c r="Y89">
         <v>0</v>
       </c>
+      <c r="Z89">
+        <f>IF(B89="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA89">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB89">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z89*3+1)*(R89*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="B90" t="s">
@@ -8361,18 +8339,18 @@
       <c r="Y90">
         <v>0</v>
       </c>
+      <c r="Z90">
+        <f>IF(B90="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA90">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB90">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z90*3+1)*(R90*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="B91" t="s">
@@ -8435,18 +8413,18 @@
       <c r="Y91">
         <v>0</v>
       </c>
+      <c r="Z91">
+        <f>IF(B91="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA91">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB91">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z91*3+1)*(R91*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>91</v>
       </c>
       <c r="B92" t="s">
@@ -8506,18 +8484,18 @@
       <c r="Y92">
         <v>1</v>
       </c>
+      <c r="Z92">
+        <f>IF(B92="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA92">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB92">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z92*3+1)*(R92*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="B93" t="s">
@@ -8580,18 +8558,18 @@
       <c r="Y93">
         <v>1</v>
       </c>
+      <c r="Z93">
+        <f>IF(B93="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA93">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB93">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+        <f>(Z93*3+1)*(R93*3+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
       <c r="B94" t="s">
@@ -8654,12 +8632,12 @@
       <c r="Y94">
         <v>1</v>
       </c>
+      <c r="Z94">
+        <f>IF(B94="movement",1,0)</f>
+        <v>0</v>
+      </c>
       <c r="AA94">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB94">
-        <f t="shared" si="5"/>
+        <f>(Z94*3+1)*(R94*3+1)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>